<commit_message>
Documentos finales de gestion
</commit_message>
<xml_diff>
--- a/proyecto/iteraciones/Product BackLog.xlsx
+++ b/proyecto/iteraciones/Product BackLog.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Auxiliar" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="147">
   <si>
     <t>Prioridad</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>Informacion del diseño de examen en la correccion</t>
+  </si>
+  <si>
+    <t>Ejecutar Ciclos de Test</t>
   </si>
 </sst>
 </file>
@@ -923,13 +926,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B3:J142" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="B3:J142">
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="En desarrollo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B3:J142"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Historia" dataDxfId="8"/>
     <tableColumn id="2" name="Instancia" dataDxfId="7"/>
@@ -1240,7 +1237,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1250,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112:F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1327,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -1360,7 +1357,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
         <f>A4+1</f>
         <v>2</v>
@@ -1391,7 +1388,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="23">
         <f t="shared" ref="A6:A69" si="0">A5+1</f>
         <v>3</v>
@@ -1422,7 +1419,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1451,7 +1448,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1482,7 +1479,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1513,7 +1510,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1544,7 +1541,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1575,7 +1572,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1606,7 +1603,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1637,7 +1634,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1670,7 +1667,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1703,7 +1700,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1736,7 +1733,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1769,7 +1766,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1802,7 +1799,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1835,7 +1832,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1868,7 +1865,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1901,7 +1898,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1934,7 +1931,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1967,7 +1964,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2000,7 +1997,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2033,7 +2030,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2066,7 +2063,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2099,7 +2096,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2132,7 +2129,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2165,7 +2162,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2198,7 +2195,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2231,7 +2228,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2264,7 +2261,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2297,7 +2294,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="32.25" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2330,7 +2327,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2363,7 +2360,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2396,7 +2393,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2429,7 +2426,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2462,7 +2459,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2495,7 +2492,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2528,7 +2525,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2561,7 +2558,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2594,7 +2591,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2627,7 +2624,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="23">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2660,7 +2657,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="23">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2693,7 +2690,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="23">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2726,7 +2723,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="23">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2759,7 +2756,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="23">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2792,7 +2789,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="23">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2825,7 +2822,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="23">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2858,7 +2855,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2891,7 +2888,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2924,7 +2921,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2957,7 +2954,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="23">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2990,7 +2987,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="23">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3058,7 +3055,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="23">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3091,7 +3088,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="23">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3124,7 +3121,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3157,7 +3154,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="23">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -3190,7 +3187,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="23">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -3256,7 +3253,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="23">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3289,7 +3286,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="23">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3322,7 +3319,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="23">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -3355,7 +3352,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="23">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -3388,7 +3385,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="23">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -3421,7 +3418,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="23">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -3453,7 +3450,7 @@
       <c r="J68" s="12"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="23">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3484,7 +3481,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="23">
         <f t="shared" ref="A70:A133" si="1">A69+1</f>
         <v>67</v>
@@ -3515,7 +3512,7 @@
       </c>
       <c r="J70" s="12"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="23">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -3544,7 +3541,7 @@
       </c>
       <c r="J71" s="12"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="23">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -3573,7 +3570,7 @@
       </c>
       <c r="J72" s="12"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="23">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -3604,7 +3601,7 @@
       </c>
       <c r="J73" s="12"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="23">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -3666,7 +3663,7 @@
       </c>
       <c r="J75" s="12"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="23">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -3697,7 +3694,7 @@
       </c>
       <c r="J76" s="12"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="23">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -3728,7 +3725,7 @@
       </c>
       <c r="J77" s="12"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="23">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -3759,7 +3756,7 @@
       </c>
       <c r="J78" s="12"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="23">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -3790,7 +3787,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="23">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -3819,7 +3816,7 @@
       </c>
       <c r="J80" s="12"/>
     </row>
-    <row r="81" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="23">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -3850,7 +3847,7 @@
       </c>
       <c r="J81" s="12"/>
     </row>
-    <row r="82" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="23">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -3881,7 +3878,7 @@
       </c>
       <c r="J82" s="12"/>
     </row>
-    <row r="83" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="23">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -3912,7 +3909,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="23">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -3943,7 +3940,7 @@
       </c>
       <c r="J84" s="12"/>
     </row>
-    <row r="85" spans="1:10" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A85" s="23">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -3976,7 +3973,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="23">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -4007,7 +4004,7 @@
       </c>
       <c r="J86" s="12"/>
     </row>
-    <row r="87" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="23">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -4038,7 +4035,7 @@
       </c>
       <c r="J87" s="12"/>
     </row>
-    <row r="88" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="23">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -4069,7 +4066,7 @@
       </c>
       <c r="J88" s="12"/>
     </row>
-    <row r="89" spans="1:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A89" s="23">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -4100,7 +4097,7 @@
       </c>
       <c r="J89" s="12"/>
     </row>
-    <row r="90" spans="1:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="23">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -4131,7 +4128,7 @@
       </c>
       <c r="J90" s="12"/>
     </row>
-    <row r="91" spans="1:10" ht="63" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A91" s="23">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -4193,7 +4190,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="23">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -4224,7 +4221,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="23">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -4255,7 +4252,7 @@
       </c>
       <c r="J94" s="12"/>
     </row>
-    <row r="95" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="23">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -4286,7 +4283,7 @@
       </c>
       <c r="J95" s="12"/>
     </row>
-    <row r="96" spans="1:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A96" s="23">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -4317,7 +4314,7 @@
       </c>
       <c r="J96" s="12"/>
     </row>
-    <row r="97" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="23">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -4348,7 +4345,7 @@
       </c>
       <c r="J97" s="12"/>
     </row>
-    <row r="98" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="23">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -4379,7 +4376,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="23">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -4410,7 +4407,7 @@
       </c>
       <c r="J99" s="12"/>
     </row>
-    <row r="100" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="23">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -4439,7 +4436,7 @@
       <c r="I100" s="14"/>
       <c r="J100" s="12"/>
     </row>
-    <row r="101" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="23">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -4468,7 +4465,7 @@
       <c r="I101" s="14"/>
       <c r="J101" s="12"/>
     </row>
-    <row r="102" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="23">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -4497,7 +4494,7 @@
       <c r="I102" s="14"/>
       <c r="J102" s="12"/>
     </row>
-    <row r="103" spans="1:10" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="23">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4555,7 +4552,7 @@
       <c r="I104" s="14"/>
       <c r="J104" s="12"/>
     </row>
-    <row r="105" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="23">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4584,7 +4581,7 @@
       <c r="I105" s="14"/>
       <c r="J105" s="12"/>
     </row>
-    <row r="106" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="23">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4613,7 +4610,7 @@
       <c r="I106" s="14"/>
       <c r="J106" s="12"/>
     </row>
-    <row r="107" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="23">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4642,7 +4639,7 @@
       <c r="I107" s="14"/>
       <c r="J107" s="12"/>
     </row>
-    <row r="108" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="23">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4671,7 +4668,7 @@
       <c r="I108" s="14"/>
       <c r="J108" s="12"/>
     </row>
-    <row r="109" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="23">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4700,7 +4697,7 @@
       </c>
       <c r="J109" s="12"/>
     </row>
-    <row r="110" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="23">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4729,7 +4726,7 @@
       <c r="I110" s="14"/>
       <c r="J110" s="12"/>
     </row>
-    <row r="111" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="23">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4758,7 +4755,7 @@
       </c>
       <c r="J111" s="12"/>
     </row>
-    <row r="112" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="23">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4787,7 +4784,7 @@
       </c>
       <c r="J112" s="12"/>
     </row>
-    <row r="113" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="23">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4816,7 +4813,7 @@
       <c r="I113" s="14"/>
       <c r="J113" s="12"/>
     </row>
-    <row r="114" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="23">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4845,7 +4842,7 @@
       </c>
       <c r="J114" s="12"/>
     </row>
-    <row r="115" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="23">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4874,7 +4871,7 @@
       <c r="I115" s="14"/>
       <c r="J115" s="12"/>
     </row>
-    <row r="116" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="23">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4968,13 +4965,27 @@
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="B119" s="12"/>
-      <c r="C119" s="13"/>
-      <c r="D119" s="13"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="13"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
+      <c r="B119" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D119" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F119" s="13">
+        <v>5</v>
+      </c>
+      <c r="G119" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H119" s="13">
+        <v>22</v>
+      </c>
       <c r="I119" s="14"/>
       <c r="J119" s="12"/>
     </row>

</xml_diff>